<commit_message>
Compare images fail test cases Added
</commit_message>
<xml_diff>
--- a/InputFiles/MultiligualTestData.xlsx
+++ b/InputFiles/MultiligualTestData.xlsx
@@ -744,7 +744,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,7 +753,7 @@
     <col min="2" max="2" width="47.140625" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
     <col min="7" max="7" width="38.140625" customWidth="1"/>
     <col min="8" max="8" width="30.7109375" customWidth="1"/>

</xml_diff>

<commit_message>
Remove the facebook test cases
</commit_message>
<xml_diff>
--- a/InputFiles/MultiligualTestData.xlsx
+++ b/InputFiles/MultiligualTestData.xlsx
@@ -761,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>